<commit_message>
improving the send_reminder file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -476,11 +476,11 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Reminded</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45932</v>
+        <v>45954</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -526,11 +526,11 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45933</v>
+        <v>45954</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Reminded</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,11 +551,11 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45934</v>
+        <v>45954</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Reminded</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>